<commit_message>
Day 09: HTML special chars
</commit_message>
<xml_diff>
--- a/Batch-02-May-2020/CS02-Day-07-08- Using Tables/table-examples.xlsx
+++ b/Batch-02-May-2020/CS02-Day-07-08- Using Tables/table-examples.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t xml:space="preserve">Sr. No</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t xml:space="preserve">Row 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student List</t>
   </si>
   <si>
     <t xml:space="preserve">Full Name</t>
@@ -140,6 +143,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -160,29 +164,34 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="15"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -255,7 +264,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -290,6 +299,10 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -390,7 +403,7 @@
   <sheetFormatPr defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.19"/>
@@ -558,139 +571,144 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="27.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="26.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="26.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="8" width="11.52"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="31.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
+      <c r="A2" s="10" t="s">
         <v>22</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="B3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="11"/>
       <c r="E3" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>27</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11" t="s">
+      <c r="A5" s="12" t="s">
         <v>29</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11" t="s">
-        <v>29</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11" t="s">
-        <v>29</v>
+      <c r="A7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11" t="s">
-        <v>29</v>
+      <c r="A8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11" t="s">
-        <v>29</v>
+      <c r="A9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11" t="s">
-        <v>29</v>
+      <c r="A10" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
     </row>
     <row r="12" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -698,7 +716,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>